<commit_message>
Woops I did it again
</commit_message>
<xml_diff>
--- a/SpeicherBelegungen.xlsx
+++ b/SpeicherBelegungen.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
   <si>
     <t>r0</t>
   </si>
@@ -122,15 +122,6 @@
     <t>imagepixelIndex</t>
   </si>
   <si>
-    <t>rValue</t>
-  </si>
-  <si>
-    <t>bValue</t>
-  </si>
-  <si>
-    <t>gValue</t>
-  </si>
-  <si>
     <t>calc Index 1</t>
   </si>
   <si>
@@ -228,16 +219,52 @@
   </si>
   <si>
     <t>colorValue</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>s10</t>
+  </si>
+  <si>
+    <t>s11</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>last pointer new array</t>
+  </si>
+  <si>
+    <t>d8</t>
+  </si>
+  <si>
+    <t>d9</t>
+  </si>
+  <si>
+    <t>d10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -275,10 +302,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -593,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6090BCA7-DA4C-4993-ADE1-700C25FC9332}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,19 +637,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -634,7 +663,7 @@
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -642,13 +671,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -659,24 +688,21 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -684,27 +710,24 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -715,10 +738,10 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -729,13 +752,13 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -746,16 +769,16 @@
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -766,13 +789,13 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -780,10 +803,10 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="G13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -791,7 +814,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -799,7 +822,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -863,7 +886,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -871,7 +894,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -879,8 +902,81 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
-      </c>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Commandline Input, windowImage SISD part
</commit_message>
<xml_diff>
--- a/SpeicherBelegungen.xlsx
+++ b/SpeicherBelegungen.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
   <si>
     <t>r0</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>d10</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nebenrechnungen </t>
   </si>
 </sst>
 </file>
@@ -625,7 +631,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,6 +729,9 @@
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
       <c r="D8" t="s">
         <v>41</v>
       </c>
@@ -822,7 +831,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Shitton of stuff (see description)
Changed names to window & zoom to reflect assignment. Ported first half of zoom to SIMD. (Currently broken.) Added time measuring to main.c for all three versions. (Also broken, sometimes gives negative values)
</commit_message>
<xml_diff>
--- a/SpeicherBelegungen.xlsx
+++ b/SpeicherBelegungen.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
   <si>
     <t>r0</t>
   </si>
@@ -255,6 +255,48 @@
   </si>
   <si>
     <t xml:space="preserve">Nebenrechnungen </t>
+  </si>
+  <si>
+    <t>Zwischenspeichern</t>
+  </si>
+  <si>
+    <t>q0</t>
+  </si>
+  <si>
+    <t>q1</t>
+  </si>
+  <si>
+    <t>q2</t>
+  </si>
+  <si>
+    <t>q3</t>
+  </si>
+  <si>
+    <t>q4</t>
+  </si>
+  <si>
+    <t>pixelX</t>
+  </si>
+  <si>
+    <t>pixelY</t>
+  </si>
+  <si>
+    <t>windowWidth</t>
+  </si>
+  <si>
+    <t>q5</t>
+  </si>
+  <si>
+    <t>q6</t>
+  </si>
+  <si>
+    <t>q7</t>
+  </si>
+  <si>
+    <t>immediates</t>
+  </si>
+  <si>
+    <t>size of new image (in bytes)</t>
   </si>
 </sst>
 </file>
@@ -276,7 +318,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,6 +337,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -308,12 +356,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -630,14 +679,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6090BCA7-DA4C-4993-ADE1-700C25FC9332}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
     <col min="7" max="7" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -825,6 +875,9 @@
       <c r="B14" t="s">
         <v>36</v>
       </c>
+      <c r="D14" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -834,15 +887,18 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -850,7 +906,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -858,7 +914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -866,7 +922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -874,7 +930,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -882,7 +938,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -890,7 +946,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -898,7 +954,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -906,7 +962,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -914,20 +970,20 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
@@ -935,7 +991,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>73</v>
       </c>
@@ -943,7 +999,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>74</v>
       </c>
@@ -951,43 +1007,75 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rewrote window.S MORE PERFORMANCE
</commit_message>
<xml_diff>
--- a/SpeicherBelegungen.xlsx
+++ b/SpeicherBelegungen.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ostne\Documents\Uni\WS 17-18\ASP\bestASP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saman\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" xr2:uid="{CD3DF208-A1A5-413D-8D7A-7E44064D6E7D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8805" xr2:uid="{CD3DF208-A1A5-413D-8D7A-7E44064D6E7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="118">
   <si>
     <t>r0</t>
   </si>
@@ -47,12 +47,6 @@
     <t>imagedata</t>
   </si>
   <si>
-    <t>xPos</t>
-  </si>
-  <si>
-    <t>yPos</t>
-  </si>
-  <si>
     <t>Width</t>
   </si>
   <si>
@@ -116,27 +110,12 @@
     <t>s9</t>
   </si>
   <si>
-    <t>og Width</t>
-  </si>
-  <si>
     <t>imagepixelIndex</t>
   </si>
   <si>
-    <t>calc Index 1</t>
-  </si>
-  <si>
-    <t>calc Index 2</t>
-  </si>
-  <si>
-    <t>immediate Value</t>
-  </si>
-  <si>
     <t>nextFree</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>WINDOW</t>
   </si>
   <si>
@@ -327,6 +306,78 @@
   </si>
   <si>
     <t>mapped Parent</t>
+  </si>
+  <si>
+    <t>FILL SIMD</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>loop y</t>
+  </si>
+  <si>
+    <t>loop x</t>
+  </si>
+  <si>
+    <t>width new</t>
+  </si>
+  <si>
+    <t>height new</t>
+  </si>
+  <si>
+    <t>q8</t>
+  </si>
+  <si>
+    <t>q9</t>
+  </si>
+  <si>
+    <t>q10</t>
+  </si>
+  <si>
+    <t>q11</t>
+  </si>
+  <si>
+    <t>q12</t>
+  </si>
+  <si>
+    <t>q13</t>
+  </si>
+  <si>
+    <t>q14</t>
+  </si>
+  <si>
+    <t>q15</t>
+  </si>
+  <si>
+    <t>Nebenrechnungen</t>
+  </si>
+  <si>
+    <t>posX</t>
+  </si>
+  <si>
+    <t>posY</t>
+  </si>
+  <si>
+    <t>parentY</t>
+  </si>
+  <si>
+    <t>out of bounds</t>
+  </si>
+  <si>
+    <t>indexParent</t>
+  </si>
+  <si>
+    <t>indexCurrent</t>
+  </si>
+  <si>
+    <t>imagedata (first index in new image; posX and posY already used)</t>
+  </si>
+  <si>
+    <t>ogWidth</t>
   </si>
 </sst>
 </file>
@@ -707,445 +758,513 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6090BCA7-DA4C-4993-ADE1-700C25FC9332}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.68359375" customWidth="1"/>
-    <col min="2" max="2" width="17.578125" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15.3125" customWidth="1"/>
-    <col min="7" max="7" width="25.83984375" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
-        <v>45</v>
-      </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>116</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>45</v>
+      </c>
+      <c r="H6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G9" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>66</v>
-      </c>
-      <c r="G13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="3"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="E36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" t="s">
+        <v>89</v>
+      </c>
+      <c r="H38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E39" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" t="s">
+        <v>90</v>
+      </c>
+      <c r="H39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" t="s">
+        <v>83</v>
+      </c>
+      <c r="F40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="5" t="s">
+      <c r="E41" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H41" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D38" t="s">
-        <v>39</v>
-      </c>
-      <c r="E38" t="s">
-        <v>88</v>
-      </c>
-      <c r="F38" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="5" t="s">
+      <c r="D42" t="s">
+        <v>78</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" t="s">
+        <v>93</v>
+      </c>
+      <c r="H42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D39" t="s">
-        <v>79</v>
-      </c>
-      <c r="E39" t="s">
-        <v>89</v>
-      </c>
-      <c r="F39" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="5" t="s">
+      <c r="F43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" t="s">
+        <v>51</v>
+      </c>
+      <c r="H43" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D40" t="s">
-        <v>80</v>
-      </c>
-      <c r="E40" t="s">
-        <v>90</v>
-      </c>
-      <c r="F40" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D41" t="s">
-        <v>81</v>
-      </c>
-      <c r="E41" t="s">
-        <v>91</v>
-      </c>
-      <c r="F41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D42" t="s">
-        <v>85</v>
-      </c>
-      <c r="F42" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" t="s">
+      <c r="F44" t="s">
+        <v>92</v>
+      </c>
+      <c r="H44" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H45" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H46" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F43" t="s">
-        <v>14</v>
-      </c>
-      <c r="G43" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F44" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="4"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="4"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="4"/>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H51" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H52" t="s">
+        <v>109</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>